<commit_message>
update Practitioner.telecom slicing discr b404bf5531a9456ce6dfdfad73237287f277c2e0
</commit_message>
<xml_diff>
--- a/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-practitioner.xlsx
+++ b/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-practitioner.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-13T08:40:33+00:00</t>
+    <t>2024-11-13T08:49:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2075,8 +2075,8 @@
     <t>Need to know how to reach a practitioner independent to any roles the practitioner may have.</t>
   </si>
   <si>
-    <t xml:space="preserve">pattern:$this}
-</t>
+    <t>pattern:system}
+exists:extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-contact-point-email-type')}</t>
   </si>
   <si>
     <t>closed</t>
@@ -3533,7 +3533,7 @@
     <col min="25" max="25" width="98.61328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="107.80859375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="89.67578125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>

<commit_message>
make emailtype mandatory d245c6a6d0c11dada4d9585aae04ad4020be47b3
</commit_message>
<xml_diff>
--- a/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-practitioner.xlsx
+++ b/nriss-patch-telecom-slicing/ig/StructureDefinition-as-dp-practitioner.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12604" uniqueCount="1020">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12603" uniqueCount="1020">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-13T08:49:07+00:00</t>
+    <t>2024-11-13T08:59:38+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -25022,11 +25022,11 @@
       </c>
       <c r="C164" s="2"/>
       <c r="D164" t="s" s="2">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="E164" s="2"/>
       <c r="F164" t="s" s="2">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G164" t="s" s="2">
         <v>85</v>
@@ -25044,14 +25044,12 @@
         <v>121</v>
       </c>
       <c r="L164" t="s" s="2">
-        <v>122</v>
+        <v>214</v>
       </c>
       <c r="M164" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N164" t="s" s="2">
-        <v>124</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="N164" s="2"/>
       <c r="O164" s="2"/>
       <c r="P164" t="s" s="2">
         <v>83</v>
@@ -25136,7 +25134,7 @@
         <v>83</v>
       </c>
       <c r="AR164" t="s" s="2">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="AS164" t="s" s="2">
         <v>83</v>
@@ -25160,7 +25158,7 @@
       </c>
       <c r="E165" s="2"/>
       <c r="F165" t="s" s="2">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G165" t="s" s="2">
         <v>100</v>

</xml_diff>